<commit_message>
changes in excel test 3a
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="87">
   <si>
     <t>TC</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>http://localhost:5000/api/test/api_key-auth/productusage-espwa</t>
+  </si>
+  <si>
+    <t>testcase03a</t>
   </si>
 </sst>
 </file>
@@ -737,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1324,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>74</v>

</xml_diff>